<commit_message>
20201011 success create splited tab xlsx data
</commit_message>
<xml_diff>
--- a/aplDesignDoc.xlsx
+++ b/aplDesignDoc.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\g_gits\diffSellect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{939A9BFC-9ACC-4A9F-906F-7A1A7705889D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2966AA5B-B673-487E-B28D-27F4488A599E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IF" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>引数</t>
     <rPh sb="0" eb="2">
@@ -40,6 +41,74 @@
     <rPh sb="4" eb="5">
       <t>メイ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ExcelWriter</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>　・WorkBook</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>OneResultWriteProcedure</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>　・Sheet</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>OpeCell</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>　・x</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>　・y</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>OperationCellUtil</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>　・OpeCell</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>　・initXpositon</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>　・initYpositon</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>　・getX</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>　・getY</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>　・incrementX</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>　・incrementY</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>OperatableCell</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>　</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -405,7 +474,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
@@ -439,4 +508,98 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00C9BF31-C4AC-4881-A96A-72DBA69BD986}">
+  <dimension ref="C4:H24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="4" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="H6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="H7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="3:8" x14ac:dyDescent="0.45">
+      <c r="E10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.45">
+      <c r="E18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.45">
+      <c r="E19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.45">
+      <c r="E20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="5:5" x14ac:dyDescent="0.45">
+      <c r="E21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="5:5" x14ac:dyDescent="0.45">
+      <c r="E22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="5:5" x14ac:dyDescent="0.45">
+      <c r="E23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="5:5" x14ac:dyDescent="0.45">
+      <c r="E24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>